<commit_message>
Updated presentation and demos
</commit_message>
<xml_diff>
--- a/reactive-programming.xlsx
+++ b/reactive-programming.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameschurchill/Documents/GitHub/reactive-programming-with-rxjs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameschurchill/Documents/GitHub/utahjs-reactive-programming-with-rxjs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>1) We can have cells that contain values and other cells that are based upon those values</t>
   </si>
@@ -36,12 +36,6 @@
   </si>
   <si>
     <t>4) We simply "declare" our problem, and we don't worry about how the spreadsheet accomplishes the results</t>
-  </si>
-  <si>
-    <t>Observable</t>
-  </si>
-  <si>
-    <t>Observer or Subscriber</t>
   </si>
 </sst>
 </file>
@@ -366,24 +360,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2">
         <f>A2+B2</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>